<commit_message>
cambios alan importado de csv
</commit_message>
<xml_diff>
--- a/PresentaciónFinal/tablas cargadas/materias carreras facultad.xlsx
+++ b/PresentaciónFinal/tablas cargadas/materias carreras facultad.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SGBD\htdocs\ProgresoJunioBrenda\tablas cargadas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SGBD\htdocs\PresentaciónFinal\PresentaciónFinal\tablas cargadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61379E14-D3C6-4972-8177-2253728A137F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF671E44-1C19-4979-B685-BDB02F823990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28560" yWindow="375" windowWidth="28125" windowHeight="13920" xr2:uid="{92099D5C-0565-4B0D-8603-B4D20571E025}"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="28125" windowHeight="13920" xr2:uid="{92099D5C-0565-4B0D-8603-B4D20571E025}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1042,7 +1042,7 @@
   <dimension ref="A1:V38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V21" sqref="V2:V21"/>
+      <selection activeCell="J29" sqref="J29:J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1817,10 +1817,10 @@
         <v>145</v>
       </c>
       <c r="J29" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="O29">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
@@ -1849,10 +1849,10 @@
         <v>147</v>
       </c>
       <c r="J31" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="O31">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
@@ -1864,10 +1864,10 @@
         <v>148</v>
       </c>
       <c r="J32" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="O32">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1925,13 +1925,10 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J29:O32">
+    <sortCondition ref="O29:O32"/>
+  </sortState>
   <mergeCells count="13">
-    <mergeCell ref="N2:N9"/>
-    <mergeCell ref="N10:N17"/>
-    <mergeCell ref="N18:N25"/>
-    <mergeCell ref="T2:T8"/>
-    <mergeCell ref="T9:T15"/>
-    <mergeCell ref="T16:T21"/>
     <mergeCell ref="A2:A12"/>
     <mergeCell ref="A13:A22"/>
     <mergeCell ref="A23:A30"/>
@@ -1939,6 +1936,12 @@
     <mergeCell ref="G2:G10"/>
     <mergeCell ref="G11:G18"/>
     <mergeCell ref="G19:G25"/>
+    <mergeCell ref="N2:N9"/>
+    <mergeCell ref="N10:N17"/>
+    <mergeCell ref="N18:N25"/>
+    <mergeCell ref="T2:T8"/>
+    <mergeCell ref="T9:T15"/>
+    <mergeCell ref="T16:T21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>